<commit_message>
feat: params.py and optimization
</commit_message>
<xml_diff>
--- a/PRJ-23/Otimização/Resultados/pareto_points_comparison.xlsx
+++ b/PRJ-23/Otimização/Resultados/pareto_points_comparison.xlsx
@@ -453,31 +453,31 @@
         <v>10</v>
       </c>
       <c r="B2">
-        <v>9.131278789151144</v>
+        <v>7.931101374082118</v>
       </c>
       <c r="C2">
-        <v>97.77865293389127</v>
+        <v>86.07009715589497</v>
       </c>
       <c r="D2">
-        <v>0.1608945784002724</v>
+        <v>0.3490658686346772</v>
       </c>
       <c r="E2">
-        <v>1.300000029957978</v>
+        <v>1.300000029006114</v>
       </c>
       <c r="F2">
-        <v>1.010747630654421</v>
+        <v>2.891420496018723</v>
       </c>
       <c r="G2">
-        <v>15.58709889115745</v>
+        <v>16.86582474777029</v>
       </c>
       <c r="H2">
-        <v>3.568935015911306</v>
+        <v>2.614775582376851</v>
       </c>
       <c r="I2">
-        <v>420720.5442668812</v>
+        <v>432910.6052091804</v>
       </c>
       <c r="J2">
-        <v>83470.08766385422</v>
+        <v>90353.29716708262</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -485,31 +485,31 @@
         <v>11</v>
       </c>
       <c r="B3">
-        <v>11.20372356376084</v>
+        <v>8.54382572435529</v>
       </c>
       <c r="C3">
-        <v>90.8286361267721</v>
+        <v>83.10702688585363</v>
       </c>
       <c r="D3">
-        <v>0.1749622321359105</v>
+        <v>0.3490659540409425</v>
       </c>
       <c r="E3">
-        <v>1.300000246363643</v>
+        <v>1.300000138478478</v>
       </c>
       <c r="F3">
-        <v>1.019332880813949</v>
+        <v>2.625616941278975</v>
       </c>
       <c r="G3">
-        <v>15.50744428130874</v>
+        <v>16.87188917665214</v>
       </c>
       <c r="H3">
-        <v>3.59672403479103</v>
+        <v>3.006381090403016</v>
       </c>
       <c r="I3">
-        <v>421429.5764373142</v>
+        <v>433068.4904151663</v>
       </c>
       <c r="J3">
-        <v>80455.81369604729</v>
+        <v>89058.25325098043</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -517,31 +517,31 @@
         <v>12</v>
       </c>
       <c r="B4">
-        <v>11.99999690542415</v>
+        <v>8.841546974461503</v>
       </c>
       <c r="C4">
-        <v>99.95250326534497</v>
+        <v>81.84032742085405</v>
       </c>
       <c r="D4">
-        <v>0.1592979759462105</v>
+        <v>0.3490659069668735</v>
       </c>
       <c r="E4">
-        <v>1.300000026948509</v>
+        <v>1.300000021654077</v>
       </c>
       <c r="F4">
-        <v>1.070132645601856</v>
+        <v>2.587215045781068</v>
       </c>
       <c r="G4">
-        <v>15.58644701129661</v>
+        <v>16.86284157260362</v>
       </c>
       <c r="H4">
-        <v>3.182927994112205</v>
+        <v>2.600187315528718</v>
       </c>
       <c r="I4">
-        <v>423467.2273470694</v>
+        <v>433226.0048153992</v>
       </c>
       <c r="J4">
-        <v>79204.56493286688</v>
+        <v>88485.25331105404</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: convergence in  multi_objetivo.py
</commit_message>
<xml_diff>
--- a/PRJ-23/Otimização/Resultados/pareto_points_comparison.xlsx
+++ b/PRJ-23/Otimização/Resultados/pareto_points_comparison.xlsx
@@ -46,13 +46,13 @@
     <t>Wf</t>
   </si>
   <si>
-    <t>Ponto A</t>
-  </si>
-  <si>
-    <t>Ponto B</t>
-  </si>
-  <si>
-    <t>Ponto C</t>
+    <t>Mínimo Peso</t>
+  </si>
+  <si>
+    <t>Escolha Otimizada</t>
+  </si>
+  <si>
+    <t>Mínimo Combustível</t>
   </si>
 </sst>
 </file>
@@ -456,28 +456,28 @@
         <v>7.931101374082118</v>
       </c>
       <c r="C2">
-        <v>86.07009715589497</v>
+        <v>86.07238482512926</v>
       </c>
       <c r="D2">
-        <v>0.3490658686346772</v>
+        <v>0.3490658513780985</v>
       </c>
       <c r="E2">
-        <v>1.300000029006114</v>
+        <v>1.300000003857622</v>
       </c>
       <c r="F2">
-        <v>2.891420496018723</v>
+        <v>2.895051400943679</v>
       </c>
       <c r="G2">
-        <v>16.86582474777029</v>
+        <v>16.86583845168331</v>
       </c>
       <c r="H2">
-        <v>2.614775582376851</v>
+        <v>3.154140467218676</v>
       </c>
       <c r="I2">
-        <v>432910.6052091804</v>
+        <v>432909.3293292762</v>
       </c>
       <c r="J2">
-        <v>90353.29716708262</v>
+        <v>90352.61100035181</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -485,31 +485,31 @@
         <v>11</v>
       </c>
       <c r="B3">
-        <v>8.54382572435529</v>
+        <v>8.528663033692741</v>
       </c>
       <c r="C3">
-        <v>83.10702688585363</v>
+        <v>83.18084226035393</v>
       </c>
       <c r="D3">
-        <v>0.3490659540409425</v>
+        <v>0.349065862597717</v>
       </c>
       <c r="E3">
-        <v>1.300000138478478</v>
+        <v>1.300000010134926</v>
       </c>
       <c r="F3">
-        <v>2.625616941278975</v>
+        <v>2.648076555419915</v>
       </c>
       <c r="G3">
-        <v>16.87188917665214</v>
+        <v>16.87167739886053</v>
       </c>
       <c r="H3">
-        <v>3.006381090403016</v>
+        <v>3.088895628162059</v>
       </c>
       <c r="I3">
-        <v>433068.4904151663</v>
+        <v>433058.2304332009</v>
       </c>
       <c r="J3">
-        <v>89058.25325098043</v>
+        <v>89086.4875643347</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -517,31 +517,31 @@
         <v>12</v>
       </c>
       <c r="B4">
-        <v>8.841546974461503</v>
+        <v>8.844786227746354</v>
       </c>
       <c r="C4">
-        <v>81.84032742085405</v>
+        <v>81.82619516573769</v>
       </c>
       <c r="D4">
-        <v>0.3490659069668735</v>
+        <v>0.3490658504446191</v>
       </c>
       <c r="E4">
-        <v>1.300000021654077</v>
+        <v>1.300000000179947</v>
       </c>
       <c r="F4">
-        <v>2.587215045781068</v>
+        <v>2.585529403938836</v>
       </c>
       <c r="G4">
-        <v>16.86284157260362</v>
+        <v>16.86409831317507</v>
       </c>
       <c r="H4">
-        <v>2.600187315528718</v>
+        <v>3.089032205755485</v>
       </c>
       <c r="I4">
-        <v>433226.0048153992</v>
+        <v>433228.3717831786</v>
       </c>
       <c r="J4">
-        <v>88485.25331105404</v>
+        <v>88479.43131776039</v>
       </c>
     </row>
   </sheetData>

</xml_diff>